<commit_message>
Test su interfaccia, da aggiustare; Inserimento controli 3 g da crontrollare queello sulle celle
</commit_message>
<xml_diff>
--- a/CDR_CE_LT068_WCDMA_MODERNIZATION_ver2.xlsx
+++ b/CDR_CE_LT068_WCDMA_MODERNIZATION_ver2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcroot\Desktop\CE_LT_03\CDR TINA\LT068\LT068New\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\CheckCDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Appoggio" sheetId="52" state="hidden" r:id="rId1"/>
@@ -1894,7 +1894,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="450">
   <si>
     <t>BO08RNC</t>
   </si>
@@ -14646,9 +14646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12:F26"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18559,11 +18558,11 @@
   <sheetPr>
     <tabColor indexed="19"/>
   </sheetPr>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:J61"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -18677,7 +18676,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="190" t="str">
-        <f t="shared" ref="B3:B61" si="0">E3</f>
+        <f t="shared" ref="B3:B60" si="0">E3</f>
         <v>RM18RNC</v>
       </c>
       <c r="C3" s="192" t="str">
@@ -21294,50 +21293,153 @@
       </c>
     </row>
     <row r="61" spans="1:14" ht="15">
-      <c r="A61" s="156">
-        <v>15</v>
-      </c>
-      <c r="B61" s="190" t="str">
-        <f t="shared" si="0"/>
-        <v>RM18RNC</v>
-      </c>
-      <c r="C61" s="192" t="str">
-        <f>LEFT('RBS Dataset-1'!$C$3,5)&amp;M61</f>
-        <v>LT068W3</v>
-      </c>
-      <c r="D61" s="192" t="str">
-        <f>LEFT('RBS Dataset-1'!$C$3,5)&amp;N61</f>
-        <v>LT068V3</v>
-      </c>
-      <c r="E61" s="192" t="str">
-        <f>'RNC Dataset-1'!$C$3</f>
-        <v>RM18RNC</v>
-      </c>
-      <c r="F61" s="156">
-        <v>0</v>
-      </c>
-      <c r="G61" s="156">
-        <v>0</v>
-      </c>
-      <c r="H61" s="156">
-        <v>0</v>
-      </c>
-      <c r="I61" s="218" t="s">
-        <v>448</v>
-      </c>
-      <c r="J61" s="218" t="s">
-        <v>448</v>
-      </c>
+      <c r="A61" s="156"/>
+      <c r="B61" s="190"/>
+      <c r="C61" s="192"/>
+      <c r="D61" s="192"/>
+      <c r="E61" s="192"/>
+      <c r="F61" s="156"/>
+      <c r="G61" s="156"/>
+      <c r="H61" s="156"/>
+      <c r="I61" s="218"/>
+      <c r="J61" s="218"/>
       <c r="K61" s="156"/>
-      <c r="L61" s="155" t="s">
-        <v>159</v>
-      </c>
-      <c r="M61" s="177" t="s">
-        <v>158</v>
-      </c>
-      <c r="N61" s="177" t="s">
-        <v>155</v>
-      </c>
+      <c r="L61" s="155"/>
+    </row>
+    <row r="62" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A62" s="156"/>
+      <c r="B62" s="190"/>
+      <c r="C62" s="192"/>
+      <c r="D62" s="192"/>
+      <c r="E62" s="192"/>
+      <c r="F62" s="156"/>
+      <c r="G62" s="156"/>
+      <c r="H62" s="156"/>
+      <c r="I62" s="218"/>
+      <c r="J62" s="218"/>
+      <c r="K62" s="156"/>
+      <c r="M62" s="177"/>
+      <c r="N62" s="177"/>
+    </row>
+    <row r="63" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A63" s="156"/>
+      <c r="B63" s="190"/>
+      <c r="C63" s="192"/>
+      <c r="D63" s="192"/>
+      <c r="E63" s="192"/>
+      <c r="F63" s="156"/>
+      <c r="G63" s="156"/>
+      <c r="H63" s="156"/>
+      <c r="I63" s="218"/>
+      <c r="J63" s="218"/>
+      <c r="K63" s="156"/>
+      <c r="M63" s="177"/>
+      <c r="N63" s="177"/>
+    </row>
+    <row r="64" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A64" s="156"/>
+      <c r="B64" s="190"/>
+      <c r="C64" s="192"/>
+      <c r="D64" s="192"/>
+      <c r="E64" s="192"/>
+      <c r="F64" s="156"/>
+      <c r="G64" s="156"/>
+      <c r="H64" s="156"/>
+      <c r="I64" s="218"/>
+      <c r="J64" s="218"/>
+      <c r="K64" s="156"/>
+      <c r="M64" s="177"/>
+      <c r="N64" s="177"/>
+    </row>
+    <row r="65" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A65" s="156"/>
+      <c r="B65" s="190"/>
+      <c r="C65" s="192"/>
+      <c r="D65" s="192"/>
+      <c r="E65" s="192"/>
+      <c r="F65" s="156"/>
+      <c r="G65" s="156"/>
+      <c r="H65" s="156"/>
+      <c r="I65" s="218"/>
+      <c r="J65" s="218"/>
+      <c r="K65" s="156"/>
+      <c r="M65" s="177"/>
+      <c r="N65" s="177"/>
+    </row>
+    <row r="66" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A66" s="156"/>
+      <c r="B66" s="190"/>
+      <c r="C66" s="192"/>
+      <c r="D66" s="192"/>
+      <c r="E66" s="192"/>
+      <c r="F66" s="156"/>
+      <c r="G66" s="156"/>
+      <c r="H66" s="156"/>
+      <c r="I66" s="218"/>
+      <c r="J66" s="218"/>
+      <c r="K66" s="156"/>
+      <c r="M66" s="177"/>
+      <c r="N66" s="177"/>
+    </row>
+    <row r="67" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A67" s="156"/>
+      <c r="B67" s="190"/>
+      <c r="C67" s="192"/>
+      <c r="D67" s="192"/>
+      <c r="E67" s="192"/>
+      <c r="F67" s="156"/>
+      <c r="G67" s="156"/>
+      <c r="H67" s="156"/>
+      <c r="I67" s="218"/>
+      <c r="J67" s="218"/>
+      <c r="K67" s="156"/>
+      <c r="M67" s="177"/>
+      <c r="N67" s="177"/>
+    </row>
+    <row r="68" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A68" s="156"/>
+      <c r="B68" s="190"/>
+      <c r="C68" s="192"/>
+      <c r="D68" s="192"/>
+      <c r="E68" s="192"/>
+      <c r="F68" s="156"/>
+      <c r="G68" s="156"/>
+      <c r="H68" s="156"/>
+      <c r="I68" s="218"/>
+      <c r="J68" s="218"/>
+      <c r="K68" s="156"/>
+      <c r="M68" s="177"/>
+      <c r="N68" s="177"/>
+    </row>
+    <row r="69" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A69" s="156"/>
+      <c r="B69" s="190"/>
+      <c r="C69" s="192"/>
+      <c r="D69" s="192"/>
+      <c r="E69" s="192"/>
+      <c r="F69" s="156"/>
+      <c r="G69" s="156"/>
+      <c r="H69" s="156"/>
+      <c r="I69" s="218"/>
+      <c r="J69" s="218"/>
+      <c r="K69" s="156"/>
+      <c r="M69" s="177"/>
+      <c r="N69" s="177"/>
+    </row>
+    <row r="70" spans="1:14" s="155" customFormat="1" ht="15">
+      <c r="A70" s="156"/>
+      <c r="B70" s="190"/>
+      <c r="C70" s="192"/>
+      <c r="D70" s="192"/>
+      <c r="E70" s="192"/>
+      <c r="F70" s="156"/>
+      <c r="G70" s="156"/>
+      <c r="H70" s="156"/>
+      <c r="I70" s="218"/>
+      <c r="J70" s="218"/>
+      <c r="K70" s="156"/>
+      <c r="M70" s="177"/>
+      <c r="N70" s="177"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N61"/>
@@ -21356,9 +21458,9 @@
   </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G58"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>